<commit_message>
Removed bad decimals from excel file
</commit_message>
<xml_diff>
--- a/src/images/values.xlsx
+++ b/src/images/values.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12780" windowHeight="3960"/>
   </bookViews>
   <sheets>
     <sheet name="valss" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="7">
   <si>
     <t xml:space="preserve"> -</t>
   </si>
@@ -26,6 +27,15 @@
   </si>
   <si>
     <t xml:space="preserve"> *</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -856,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,16 +979,16 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E7">
-        <v>0.76919999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1054,16 +1064,16 @@
         <v>12</v>
       </c>
       <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>11</v>
-      </c>
       <c r="E12">
-        <v>0.90910000000000002</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1207,16 +1217,16 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>2.375</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1275,16 +1285,16 @@
         <v>25</v>
       </c>
       <c r="B25">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <v>18</v>
-      </c>
       <c r="E25">
-        <v>0.27779999999999999</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1513,16 +1523,16 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D39">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E39">
-        <v>0.92859999999999998</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1547,16 +1557,16 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D41">
         <v>9</v>
       </c>
       <c r="E41">
-        <v>0.22220000000000001</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,7 +1574,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -1573,7 +1583,7 @@
         <v>8</v>
       </c>
       <c r="E42">
-        <v>2.125</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1666,16 +1676,16 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D48">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E48">
-        <v>1.8571</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1802,7 +1812,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
@@ -1811,7 +1821,7 @@
         <v>3</v>
       </c>
       <c r="E56">
-        <v>3.6667000000000001</v>
+        <v>0.66669999999999996</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1972,16 +1982,16 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C66" t="s">
         <v>3</v>
       </c>
       <c r="D66">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E66">
-        <v>238</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2023,7 +2033,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
@@ -2032,7 +2042,7 @@
         <v>9</v>
       </c>
       <c r="E69">
-        <v>2.1111</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2176,7 +2186,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C78" t="s">
         <v>2</v>
@@ -2185,7 +2195,7 @@
         <v>6</v>
       </c>
       <c r="E78">
-        <v>0.83330000000000004</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2295,16 +2305,16 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C85" t="s">
         <v>2</v>
       </c>
       <c r="D85">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E85">
-        <v>0.35709999999999997</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2312,16 +2322,16 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C86" t="s">
         <v>2</v>
       </c>
       <c r="D86">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E86">
-        <v>1.8332999999999999</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2533,16 +2543,16 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C99" t="s">
         <v>2</v>
       </c>
       <c r="D99">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E99">
-        <v>5.6666999999999996</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>